<commit_message>
Initial topic layout commit
</commit_message>
<xml_diff>
--- a/data/work_schedule.xlsx
+++ b/data/work_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F586A29-76A3-48D1-8993-7C7F29077D1F}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DA6D0623-84D5-4245-A5D2-1AB913E1EF85}"/>
   <bookViews>
     <workbookView xWindow="1185" yWindow="195" windowWidth="25950" windowHeight="15405" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>week_start_date</t>
   </si>
@@ -95,6 +95,39 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>topic_link</t>
+  </si>
+  <si>
+    <t>topics/shiny_1.html</t>
+  </si>
+  <si>
+    <t>topics/shiny_2.html</t>
+  </si>
+  <si>
+    <t>topics/shiny_4.html</t>
+  </si>
+  <si>
+    <t>topics/shiny_3.html</t>
+  </si>
+  <si>
+    <t>topics/tidyverse.html</t>
+  </si>
+  <si>
+    <t>topics/geospatial.html</t>
+  </si>
+  <si>
+    <t>topics/census.html</t>
+  </si>
+  <si>
+    <t>topics/machine_learning.html</t>
+  </si>
+  <si>
+    <t>topics/rmarkdown.html</t>
+  </si>
+  <si>
+    <t>topics/misc_questions.html</t>
   </si>
 </sst>
 </file>
@@ -468,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48762DA2-7B38-4373-94E1-F79287F51130}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -483,9 +516,10 @@
     <col min="5" max="5" width="54.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -507,8 +541,11 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -526,7 +563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -545,7 +582,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -570,7 +607,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -594,8 +631,11 @@
       <c r="G5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -619,8 +659,11 @@
       <c r="G6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -644,8 +687,11 @@
       <c r="G7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -669,8 +715,11 @@
       <c r="G8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -694,8 +743,11 @@
       <c r="G9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -719,8 +771,11 @@
       <c r="G10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -744,8 +799,11 @@
       <c r="G11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -769,8 +827,11 @@
       <c r="G12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -794,8 +855,11 @@
       <c r="G13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -816,6 +880,9 @@
       </c>
       <c r="G14" t="s">
         <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -848,21 +915,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -1046,24 +1098,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1079,4 +1129,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated schedule, moved tidyverse up
</commit_message>
<xml_diff>
--- a/data/work_schedule.xlsx
+++ b/data/work_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5468E802-B14E-460F-8949-96B12E24B230}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E7A502D-4BC9-4514-B79B-8455DE8D5264}"/>
   <bookViews>
     <workbookView xWindow="1185" yWindow="195" windowWidth="25950" windowHeight="15405" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
@@ -503,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48762DA2-7B38-4373-94E1-F79287F51130}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -625,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -634,7 +634,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -653,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
@@ -662,7 +662,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -681,7 +681,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -690,7 +690,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -709,7 +709,7 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
@@ -718,7 +718,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -737,7 +737,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
@@ -746,7 +746,7 @@
         <v>19</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -765,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -774,7 +774,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -793,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
         <v>19</v>
@@ -802,7 +802,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -821,7 +821,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -830,7 +830,7 @@
         <v>19</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -886,6 +886,46 @@
       <c r="H14" s="7" t="s">
         <v>30</v>
       </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -917,21 +957,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -1115,24 +1140,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1148,4 +1171,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Starting to draft Tidyverse module
</commit_message>
<xml_diff>
--- a/data/work_schedule.xlsx
+++ b/data/work_schedule.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E7A502D-4BC9-4514-B79B-8455DE8D5264}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C6FE11DA-C291-4637-940A-789A07F44ED2}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="195" windowWidth="25950" windowHeight="15405" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="work_schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="r_users" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>week_start_date</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Census, TIGER, and LODES data in R</t>
   </si>
   <si>
-    <t>Intro to Machine Learning in R (Regression, imputation, clustering)</t>
-  </si>
-  <si>
     <t>Question Session</t>
   </si>
   <si>
@@ -121,13 +118,64 @@
     <t>topics/census.html</t>
   </si>
   <si>
-    <t>topics/machine_learning.html</t>
-  </si>
-  <si>
     <t>topics/rmarkdown.html</t>
   </si>
   <si>
     <t>topics/misc_questions.html</t>
+  </si>
+  <si>
+    <t>GTFS data in R</t>
+  </si>
+  <si>
+    <t>topics/gtfs_data.html</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>Bryan</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>Blanc</t>
+  </si>
+  <si>
+    <t>Esther</t>
+  </si>
+  <si>
+    <t>Needham</t>
+  </si>
+  <si>
+    <t>Oren</t>
+  </si>
+  <si>
+    <t>Eshel</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Leitman</t>
+  </si>
+  <si>
+    <t>r_version</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Poirier</t>
+  </si>
+  <si>
+    <t>Tomoko</t>
+  </si>
+  <si>
+    <t>DeLaTorre</t>
   </si>
 </sst>
 </file>
@@ -178,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -189,6 +237,7 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48762DA2-7B38-4373-94E1-F79287F51130}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -544,7 +593,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -628,13 +677,13 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -656,13 +705,13 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -684,13 +733,13 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -712,13 +761,13 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -740,13 +789,13 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -768,13 +817,13 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -793,16 +842,16 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -824,13 +873,13 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -849,16 +898,16 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -875,16 +924,16 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
@@ -934,13 +983,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F563AB-E9D6-4346-B147-369F776995ED}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>